<commit_message>
Edit energy requirements for DAC
</commit_message>
<xml_diff>
--- a/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
+++ b/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\geoeng\DACD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE3E547-8294-456B-BD18-A3C25200CD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B4DA15-A5FF-4D91-BA4E-A5CD251C9157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>Sources:</t>
   </si>
@@ -359,6 +359,27 @@
   </si>
   <si>
     <t>potential</t>
+  </si>
+  <si>
+    <t>see: https://www.wri.org/insights/direct-air-capture-resource-considerations-and-costs-carbon-removal, Status of the Leading DAC Companies.</t>
+  </si>
+  <si>
+    <t>However, the largest currently operating DAC facilities use solid sorbent systems and utilize non-fossil resources at low heat (80-120 C),</t>
+  </si>
+  <si>
+    <t>Therefore, we take the heat input specified for DAC1 plants and convert to the amount of electricity needed</t>
+  </si>
+  <si>
+    <t>if supplied by a heat pump.</t>
+  </si>
+  <si>
+    <t>Percent Reduction in Fuel Use with Heat Pump</t>
+  </si>
+  <si>
+    <t>Source: indst/PIFURfE</t>
+  </si>
+  <si>
+    <t>Heat Input Required per Ton CO2 Captured, Converted to Electricity</t>
   </si>
 </sst>
 </file>
@@ -368,7 +389,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -456,7 +477,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -479,7 +500,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -554,14 +579,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>11587</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>8412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>265044</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>143350</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>146525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -590,8 +615,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4964587"/>
-          <a:ext cx="4770783" cy="3560763"/>
+          <a:off x="0" y="7487608"/>
+          <a:ext cx="5002696" cy="3414851"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -603,15 +628,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>82826</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>91109</xdr:rowOff>
+      <xdr:colOff>86001</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>87934</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>74543</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>43244</xdr:rowOff>
+      <xdr:colOff>61843</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>46420</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -640,8 +665,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4754217" y="4472609"/>
-          <a:ext cx="753717" cy="523635"/>
+          <a:off x="5627066" y="7567130"/>
+          <a:ext cx="782430" cy="508313"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -919,7 +944,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD30"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1060,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C706B8D-FB10-40CA-B025-270C2E82347D}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1192,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1224,663 +1249,742 @@
         <v>24</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>300</v>
-      </c>
-      <c r="C10">
-        <v>350</v>
+      <c r="A9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>180</v>
-      </c>
-      <c r="C11">
-        <v>200</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
+      <c r="A12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+      <c r="C14">
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>180</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>1.8</v>
       </c>
-      <c r="C16">
+      <c r="C20">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17">
+      <c r="B21">
         <v>1.3</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B22">
+      <c r="B26">
         <v>8.1</v>
       </c>
-      <c r="C22">
+      <c r="C26">
         <v>7.2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <v>5.3</v>
       </c>
-      <c r="C23">
+      <c r="C27">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="18">
+        <v>0.67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7">
+        <f>B26*(1-$B$30)</f>
+        <v>2.6729999999999996</v>
+      </c>
+      <c r="C34" s="7">
+        <f>C26*(1-$B$30)</f>
+        <v>2.3759999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="7">
+        <f>B27*(1-$B$30)</f>
+        <v>1.7489999999999997</v>
+      </c>
+      <c r="C35" s="7">
+        <f>C27*(1-$B$30)</f>
+        <v>1.452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B57">
-        <v>2045</v>
-      </c>
-      <c r="C57">
-        <v>2050</v>
-      </c>
-      <c r="D57">
-        <v>2060</v>
-      </c>
-      <c r="E57">
-        <v>2070</v>
-      </c>
-      <c r="F57">
-        <v>2080</v>
-      </c>
-      <c r="G57">
-        <v>2090</v>
-      </c>
-      <c r="H57">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
-      <c r="D58">
-        <v>20</v>
-      </c>
-      <c r="E58">
-        <v>122</v>
-      </c>
-      <c r="F58">
-        <v>388</v>
-      </c>
-      <c r="G58">
-        <v>384</v>
-      </c>
-      <c r="H58">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>5</v>
-      </c>
-      <c r="F59">
-        <v>30</v>
-      </c>
-      <c r="G59">
-        <v>35</v>
-      </c>
-      <c r="H59">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B63">
-        <v>2045</v>
-      </c>
-      <c r="C63">
-        <v>2050</v>
-      </c>
-      <c r="D63">
-        <v>2060</v>
-      </c>
-      <c r="E63">
-        <v>2070</v>
-      </c>
-      <c r="F63">
-        <v>2080</v>
-      </c>
-      <c r="G63">
-        <v>2090</v>
-      </c>
-      <c r="H63">
-        <v>2100</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64">
-        <f>B58/$B$61*30</f>
-        <v>0</v>
-      </c>
-      <c r="C64" s="7">
-        <f t="shared" ref="C64:H65" si="0">C58/$B$61*30</f>
-        <v>0.3571428571428571</v>
-      </c>
-      <c r="D64" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4285714285714284</v>
-      </c>
-      <c r="E64" s="7">
-        <f t="shared" si="0"/>
-        <v>8.7142857142857153</v>
-      </c>
-      <c r="F64" s="7">
-        <f t="shared" si="0"/>
-        <v>27.714285714285715</v>
-      </c>
-      <c r="G64" s="7">
-        <f t="shared" si="0"/>
-        <v>27.428571428571427</v>
-      </c>
-      <c r="H64" s="7">
-        <f t="shared" si="0"/>
-        <v>27.071428571428573</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65">
-        <f>B59/$B$61*30</f>
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E65" s="7">
-        <f t="shared" si="0"/>
-        <v>0.3571428571428571</v>
-      </c>
-      <c r="F65" s="7">
-        <f t="shared" si="0"/>
-        <v>2.1428571428571428</v>
-      </c>
-      <c r="G65" s="7">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="H65" s="7">
-        <f t="shared" si="0"/>
-        <v>2.8571428571428568</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>35</v>
+      <c r="B68">
+        <v>2045</v>
+      </c>
+      <c r="C68">
+        <v>2050</v>
+      </c>
+      <c r="D68">
+        <v>2060</v>
+      </c>
+      <c r="E68">
+        <v>2070</v>
+      </c>
+      <c r="F68">
+        <v>2080</v>
+      </c>
+      <c r="G68">
+        <v>2090</v>
+      </c>
+      <c r="H68">
+        <v>2100</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+      <c r="E69">
+        <v>122</v>
+      </c>
+      <c r="F69">
+        <v>388</v>
+      </c>
+      <c r="G69">
+        <v>384</v>
+      </c>
+      <c r="H69">
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>5</v>
+      </c>
+      <c r="F70">
+        <v>30</v>
+      </c>
+      <c r="G70">
+        <v>35</v>
+      </c>
+      <c r="H70">
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>2045</v>
+      </c>
+      <c r="C74">
+        <v>2050</v>
+      </c>
+      <c r="D74">
+        <v>2060</v>
+      </c>
+      <c r="E74">
+        <v>2070</v>
+      </c>
+      <c r="F74">
+        <v>2080</v>
+      </c>
+      <c r="G74">
+        <v>2090</v>
+      </c>
+      <c r="H74">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75">
+        <f>B69/$B$72*30</f>
+        <v>0</v>
+      </c>
+      <c r="C75" s="7">
+        <f t="shared" ref="C75:H76" si="0">C69/$B$72*30</f>
+        <v>0.3571428571428571</v>
+      </c>
+      <c r="D75" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714284</v>
+      </c>
+      <c r="E75" s="7">
+        <f t="shared" si="0"/>
+        <v>8.7142857142857153</v>
+      </c>
+      <c r="F75" s="7">
+        <f t="shared" si="0"/>
+        <v>27.714285714285715</v>
+      </c>
+      <c r="G75" s="7">
+        <f t="shared" si="0"/>
+        <v>27.428571428571427</v>
+      </c>
+      <c r="H75" s="7">
+        <f t="shared" si="0"/>
+        <v>27.071428571428573</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76">
+        <f>B70/$B$72*30</f>
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="7">
+        <f t="shared" si="0"/>
+        <v>0.3571428571428571</v>
+      </c>
+      <c r="F76" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="G76" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H76" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8571428571428568</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>38</v>
       </c>
-      <c r="B72">
+      <c r="B83">
         <v>19.39</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C83" t="s">
         <v>40</v>
       </c>
-      <c r="D72">
+      <c r="D83">
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>39</v>
       </c>
-      <c r="B73">
+      <c r="B84">
         <v>80</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C84" t="s">
         <v>41</v>
       </c>
-      <c r="D73">
+      <c r="D84">
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>42</v>
       </c>
-      <c r="B74" s="8">
-        <f>B72/B73</f>
+      <c r="B85" s="8">
+        <f>B83/B84</f>
         <v>0.24237500000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" s="4" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B77">
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B88">
         <v>2045</v>
       </c>
-      <c r="C77">
+      <c r="C88">
         <v>2050</v>
       </c>
-      <c r="D77">
+      <c r="D88">
         <v>2060</v>
       </c>
-      <c r="E77">
+      <c r="E88">
         <v>2070</v>
       </c>
-      <c r="F77">
+      <c r="F88">
         <v>2080</v>
       </c>
-      <c r="G77">
+      <c r="G88">
         <v>2090</v>
       </c>
-      <c r="H77">
+      <c r="H88">
         <v>2100</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>32</v>
       </c>
-      <c r="B78">
-        <f>B64*$B$74</f>
-        <v>0</v>
-      </c>
-      <c r="C78" s="7">
-        <f t="shared" ref="C78:H79" si="1">C64*$B$74</f>
+      <c r="B89">
+        <f>B75*$B$85</f>
+        <v>0</v>
+      </c>
+      <c r="C89" s="7">
+        <f t="shared" ref="C89:H90" si="1">C75*$B$85</f>
         <v>8.6562499999999987E-2</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D89" s="7">
         <f t="shared" si="1"/>
         <v>0.34624999999999995</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E89" s="7">
         <f t="shared" si="1"/>
         <v>2.1121250000000003</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F89" s="7">
         <f t="shared" si="1"/>
         <v>6.7172500000000008</v>
       </c>
-      <c r="G78" s="7">
+      <c r="G89" s="7">
         <f t="shared" si="1"/>
         <v>6.6479999999999997</v>
       </c>
-      <c r="H78" s="7">
+      <c r="H89" s="7">
         <f t="shared" si="1"/>
         <v>6.5614375000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>33</v>
       </c>
-      <c r="B79">
-        <f>B65*$B$74</f>
-        <v>0</v>
-      </c>
-      <c r="C79">
+      <c r="B90">
+        <f>B76*$B$85</f>
+        <v>0</v>
+      </c>
+      <c r="C90">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D79">
+      <c r="D90">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E90" s="7">
         <f t="shared" si="1"/>
         <v>8.6562499999999987E-2</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F90" s="7">
         <f t="shared" si="1"/>
         <v>0.51937500000000003</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G90" s="7">
         <f t="shared" si="1"/>
         <v>0.60593750000000002</v>
       </c>
-      <c r="H79" s="7">
+      <c r="H90" s="7">
         <f t="shared" si="1"/>
         <v>0.69249999999999989</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B82">
-        <v>2045</v>
-      </c>
-      <c r="C82">
-        <v>2050</v>
-      </c>
-      <c r="D82">
-        <v>2060</v>
-      </c>
-      <c r="E82">
-        <v>2070</v>
-      </c>
-      <c r="F82">
-        <v>2080</v>
-      </c>
-      <c r="G82">
-        <v>2090</v>
-      </c>
-      <c r="H82">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>46</v>
-      </c>
-      <c r="B83" s="10">
-        <f>B78*10^9</f>
-        <v>0</v>
-      </c>
-      <c r="C83" s="11">
-        <f t="shared" ref="C83:H84" si="2">C78*10^9</f>
-        <v>86562499.999999985</v>
-      </c>
-      <c r="D83" s="11">
-        <f t="shared" si="2"/>
-        <v>346249999.99999994</v>
-      </c>
-      <c r="E83" s="11">
-        <f t="shared" si="2"/>
-        <v>2112125000.0000002</v>
-      </c>
-      <c r="F83" s="11">
-        <f t="shared" si="2"/>
-        <v>6717250000.000001</v>
-      </c>
-      <c r="G83" s="11">
-        <f t="shared" si="2"/>
-        <v>6648000000</v>
-      </c>
-      <c r="H83" s="11">
-        <f t="shared" si="2"/>
-        <v>6561437500</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="10">
-        <f>B79*10^9</f>
-        <v>0</v>
-      </c>
-      <c r="C84" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D84" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E84" s="11">
-        <f t="shared" si="2"/>
-        <v>86562499.999999985</v>
-      </c>
-      <c r="F84" s="11">
-        <f t="shared" si="2"/>
-        <v>519375000.00000006</v>
-      </c>
-      <c r="G84" s="11">
-        <f t="shared" si="2"/>
-        <v>605937500</v>
-      </c>
-      <c r="H84" s="11">
-        <f t="shared" si="2"/>
-        <v>692499999.99999988</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A86" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>53</v>
-      </c>
-    </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>54</v>
-      </c>
-      <c r="B92">
-        <v>947086</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>2045</v>
+      </c>
+      <c r="C93">
+        <v>2050</v>
+      </c>
+      <c r="D93">
+        <v>2060</v>
+      </c>
+      <c r="E93">
+        <v>2070</v>
+      </c>
+      <c r="F93">
+        <v>2080</v>
+      </c>
+      <c r="G93">
+        <v>2090</v>
+      </c>
+      <c r="H93">
+        <v>2100</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>46</v>
+      </c>
+      <c r="B94" s="10">
+        <f>B89*10^9</f>
+        <v>0</v>
+      </c>
+      <c r="C94" s="11">
+        <f t="shared" ref="C94:H95" si="2">C89*10^9</f>
+        <v>86562499.999999985</v>
+      </c>
+      <c r="D94" s="11">
+        <f t="shared" si="2"/>
+        <v>346249999.99999994</v>
+      </c>
+      <c r="E94" s="11">
+        <f t="shared" si="2"/>
+        <v>2112125000.0000002</v>
+      </c>
+      <c r="F94" s="11">
+        <f t="shared" si="2"/>
+        <v>6717250000.000001</v>
+      </c>
+      <c r="G94" s="11">
+        <f t="shared" si="2"/>
+        <v>6648000000</v>
+      </c>
+      <c r="H94" s="11">
+        <f t="shared" si="2"/>
+        <v>6561437500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>47</v>
+      </c>
+      <c r="B95" s="10">
+        <f>B90*10^9</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D95" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="11">
+        <f t="shared" si="2"/>
+        <v>86562499.999999985</v>
+      </c>
+      <c r="F95" s="11">
+        <f t="shared" si="2"/>
+        <v>519375000.00000006</v>
+      </c>
+      <c r="G95" s="11">
+        <f t="shared" si="2"/>
+        <v>605937500</v>
+      </c>
+      <c r="H95" s="11">
+        <f t="shared" si="2"/>
+        <v>692499999.99999988</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103">
+        <v>947086</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2172,7 +2276,7 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2293,140 +2397,140 @@
         <v>59</v>
       </c>
       <c r="B2" s="12">
-        <f>Data!B16*Data!B92</f>
-        <v>1704754.8</v>
+        <f>(Data!B20+Data!B34)*Data!B103</f>
+        <v>4236315.6780000003</v>
       </c>
       <c r="C2" s="12">
         <f>$B2</f>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="D2" s="12">
         <f t="shared" ref="D2:AI10" si="0">$B2</f>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="E2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="F2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="G2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="H2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="I2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="J2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="K2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="L2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="M2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="N2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="O2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="P2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="Q2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="R2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="S2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="T2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="U2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="V2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="W2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="X2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="Y2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="Z2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AA2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AB2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AC2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AD2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AE2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AF2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AG2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AH2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
       <c r="AI2" s="12">
         <f t="shared" si="0"/>
-        <v>1704754.8</v>
+        <v>4236315.6780000003</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
@@ -2574,140 +2678,139 @@
         <v>61</v>
       </c>
       <c r="B4" s="12">
-        <f>Data!B22*Data!B92</f>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="1"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="D4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="E4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="G4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="H4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="I4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="J4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="K4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="L4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="M4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="N4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="P4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="R4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="S4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="T4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="U4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="V4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="W4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="X4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="12">
         <f t="shared" si="0"/>
-        <v>7671396.5999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
@@ -3822,7 +3925,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="12">
-        <f>Data!B10</f>
+        <f>Data!B14</f>
         <v>300</v>
       </c>
       <c r="C2" s="12">

</xml_diff>

<commit_message>
Allow DAC potential to begin phasing in in 2030
</commit_message>
<xml_diff>
--- a/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
+++ b/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\geoeng\DACD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\geoeng\DACD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B4DA15-A5FF-4D91-BA4E-A5CD251C9157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5139D15E-CB52-4E6B-A000-C9F7BE131494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -943,32 +943,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="47.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,97 +976,97 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>2021</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>2019</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1085,17 +1085,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C706B8D-FB10-40CA-B025-270C2E82347D}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>95</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>96</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>94</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>97</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>8.9285714285714274E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1145,42 +1145,42 @@
         <v>0.3571428571428571</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2020</v>
       </c>
       <c r="C16">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D16">
         <v>2040</v>
@@ -1189,7 +1189,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1219,62 +1219,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A36" sqref="A36:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
-    <col min="2" max="8" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>73</v>
       </c>
@@ -1285,7 +1285,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1329,12 +1329,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1367,17 +1367,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1410,15 +1410,15 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>103</v>
       </c>
@@ -1429,15 +1429,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>2.3759999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1474,27 +1474,27 @@
         <v>1.452</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>43</v>
       </c>
@@ -1506,27 +1506,27 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>2045</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>2045</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>32</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>27.071428571428573</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>33</v>
       </c>
@@ -1698,27 +1698,27 @@
         <v>2.8571428571428568</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>38</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>39</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>0.24237500000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>44</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>2045</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>32</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>6.5614375000000003</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>33</v>
       </c>
@@ -1856,12 +1856,12 @@
         <v>0.69249999999999989</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>2045</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>46</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>6561437500</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>47</v>
       </c>
@@ -1950,32 +1950,32 @@
         <v>692499999.99999988</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>54</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>947086</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>72</v>
       </c>
@@ -2006,16 +2006,16 @@
       <selection activeCell="AI2" sqref="B2:AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="24" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="35" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="35" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -2180,43 +2180,43 @@
       </c>
       <c r="O2" s="16" cm="1">
         <f t="array" ref="O2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!O1)</f>
-        <v>0</v>
+        <v>8116883.1168842316</v>
       </c>
       <c r="P2" s="16" cm="1">
         <f t="array" ref="P2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!P1)</f>
-        <v>8928571.4285736084</v>
+        <v>16233766.233766556</v>
       </c>
       <c r="Q2" s="16" cm="1">
         <f t="array" ref="Q2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!Q1)</f>
-        <v>17857142.857143402</v>
+        <v>24350649.35064888</v>
       </c>
       <c r="R2" s="16" cm="1">
         <f t="array" ref="R2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!R1)</f>
-        <v>26785714.28571701</v>
+        <v>32467532.467533112</v>
       </c>
       <c r="S2" s="16" cm="1">
         <f t="array" ref="S2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!S1)</f>
-        <v>35714285.714286804</v>
+        <v>40584415.584415436</v>
       </c>
       <c r="T2" s="16" cm="1">
         <f t="array" ref="T2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!T1)</f>
-        <v>44642857.142856598</v>
+        <v>48701298.701299667</v>
       </c>
       <c r="U2" s="16" cm="1">
         <f t="array" ref="U2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!U1)</f>
-        <v>53571428.571430206</v>
+        <v>56818181.818181992</v>
       </c>
       <c r="V2" s="16" cm="1">
         <f t="array" ref="V2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!V1)</f>
-        <v>62500000</v>
+        <v>64935064.935064316</v>
       </c>
       <c r="W2" s="16" cm="1">
         <f t="array" ref="W2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!W1)</f>
-        <v>71428571.428573608</v>
+        <v>73051948.051948547</v>
       </c>
       <c r="X2" s="16" cm="1">
         <f t="array" ref="X2">TREND('CDR potential'!$C$17:$D$17,'CDR potential'!$C$16:$D$16,'DACD-potential'!X1)</f>
-        <v>80357142.857143402</v>
+        <v>81168831.168830872</v>
       </c>
       <c r="Y2" s="16" cm="1">
         <f t="array" ref="Y2">TREND('CDR potential'!$D$17:$E$17,'CDR potential'!$D$16:$E$16,'DACD-potential'!Y1)</f>
@@ -2279,13 +2279,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>4236315.6780000003</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3807,13 +3807,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>

</xml_diff>